<commit_message>
EPBDS-11327 "class" information can't be found in the OpenL datatypes
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7544_field_access/EPBDS-7544.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7544_field_access/EPBDS-7544.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-7544_field_access\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-7544_field_access\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC9E169-F7F9-448D-B7DC-6DD56085C884}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0406C6-EFBF-481F-85B4-D501779D0C80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E59F7472-A9D2-4FC2-8ED3-4C22BD94DB84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E59F7472-A9D2-4FC2-8ED3-4C22BD94DB84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="126">
   <si>
     <t>Step</t>
   </si>
@@ -340,6 +340,69 @@
   </si>
   <si>
     <t>= AccessBean.name()</t>
+  </si>
+  <si>
+    <t>case21</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case21</t>
+  </si>
+  <si>
+    <t>SR21</t>
+  </si>
+  <si>
+    <t>AccessBean</t>
+  </si>
+  <si>
+    <t>Datatype MyType</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>case22</t>
+  </si>
+  <si>
+    <t>case23</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case22</t>
+  </si>
+  <si>
+    <t>SR22</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case23</t>
+  </si>
+  <si>
+    <t>SR23</t>
+  </si>
+  <si>
+    <t>MyType</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>case24</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case24</t>
+  </si>
+  <si>
+    <t>SR24</t>
+  </si>
+  <si>
+    <t>= new MyType().value</t>
+  </si>
+  <si>
+    <t>= new MyType().getValue()</t>
+  </si>
+  <si>
+    <t>= AccessBean.class.simpleName</t>
+  </si>
+  <si>
+    <t>= MyType.class.simpleName</t>
   </si>
 </sst>
 </file>
@@ -416,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -430,10 +493,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B72988DF-F47F-4438-80D5-32C51C31A17F}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,9 +515,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -489,7 +555,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -595,7 +661,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -745,38 +811,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DCC082-B645-4260-A0B9-5F0428966443}">
-  <dimension ref="B4:K28"/>
+  <dimension ref="B4:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
       <c r="J4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -800,7 +866,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -818,7 +884,7 @@
       </c>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -838,7 +904,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
@@ -858,7 +924,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -876,7 +942,7 @@
       </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -894,7 +960,7 @@
       </c>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
@@ -912,7 +978,7 @@
       </c>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -930,7 +996,7 @@
       </c>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
@@ -948,7 +1014,7 @@
       </c>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>27</v>
       </c>
@@ -966,7 +1032,7 @@
       </c>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
@@ -984,7 +1050,7 @@
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>38</v>
       </c>
@@ -1004,7 +1070,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>46</v>
       </c>
@@ -1024,7 +1090,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>47</v>
       </c>
@@ -1044,7 +1110,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>48</v>
       </c>
@@ -1064,7 +1130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>49</v>
       </c>
@@ -1084,7 +1150,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>50</v>
       </c>
@@ -1104,7 +1170,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>73</v>
       </c>
@@ -1122,7 +1188,7 @@
       </c>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>79</v>
       </c>
@@ -1142,7 +1208,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>89</v>
       </c>
@@ -1162,7 +1228,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>80</v>
       </c>
@@ -1182,29 +1248,117 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="1"/>
+      <c r="E27" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>